<commit_message>
16bit Comparison Instructions added
</commit_message>
<xml_diff>
--- a/hard/v0/PLsi_v0_estimated_cost.xlsx
+++ b/hard/v0/PLsi_v0_estimated_cost.xlsx
@@ -482,10 +482,10 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.38"/>
@@ -589,7 +589,7 @@
         <v>14</v>
       </c>
       <c r="K5" s="12" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L5" s="13" t="s">
         <v>15</v>
@@ -626,7 +626,7 @@
         <v>18</v>
       </c>
       <c r="K6" s="12" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L6" s="13" t="s">
         <v>19</v>
@@ -664,7 +664,7 @@
         <v>22</v>
       </c>
       <c r="K7" s="12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L7" s="13" t="s">
         <v>23</v>
@@ -702,7 +702,7 @@
         <v>25</v>
       </c>
       <c r="K8" s="12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L8" s="13" t="s">
         <v>23</v>
@@ -767,11 +767,11 @@
       </c>
       <c r="F10" s="9" t="n">
         <f aca="false">K5+K6</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G10" s="9" t="n">
         <f aca="false">E10*F10</f>
-        <v>0.07448</v>
+        <v>0.0532</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>30</v>
@@ -807,11 +807,11 @@
       </c>
       <c r="F11" s="9" t="n">
         <f aca="false">K6</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G11" s="9" t="n">
         <f aca="false">E11*F11</f>
-        <v>1.6404</v>
+        <v>1.0936</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>18</v>
@@ -866,11 +866,11 @@
       </c>
       <c r="F13" s="9" t="n">
         <f aca="false">K6</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G13" s="9" t="n">
         <f aca="false">E13*F13</f>
-        <v>0.0576</v>
+        <v>0.0384</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>34</v>
@@ -896,11 +896,11 @@
       </c>
       <c r="F14" s="9" t="n">
         <f aca="false">K5</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G14" s="9" t="n">
         <f aca="false">E14*F14</f>
-        <v>0.2192</v>
+        <v>0.1644</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>14</v>
@@ -926,11 +926,11 @@
       </c>
       <c r="F15" s="9" t="n">
         <f aca="false">K5</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15" s="9" t="n">
         <f aca="false">E15*F15</f>
-        <v>0.104</v>
+        <v>0.078</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>14</v>
@@ -956,11 +956,11 @@
       </c>
       <c r="F16" s="9" t="n">
         <f aca="false">K5</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G16" s="9" t="n">
         <f aca="false">E16*F16</f>
-        <v>0.0768</v>
+        <v>0.0576</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>14</v>
@@ -986,11 +986,11 @@
       </c>
       <c r="F17" s="9" t="n">
         <f aca="false">K5</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G17" s="9" t="n">
         <f aca="false">E17*F17</f>
-        <v>0.1408</v>
+        <v>0.1056</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>14</v>
@@ -1015,12 +1015,12 @@
         <v>0.0096</v>
       </c>
       <c r="F18" s="9" t="n">
-        <f aca="false">K5+K7*2</f>
-        <v>8</v>
+        <f aca="false">K5+K7*3+K8</f>
+        <v>14</v>
       </c>
       <c r="G18" s="9" t="n">
         <f aca="false">E18*F18</f>
-        <v>0.0768</v>
+        <v>0.1344</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>14</v>
@@ -1046,11 +1046,11 @@
       </c>
       <c r="F19" s="9" t="n">
         <f aca="false">$K$8/2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="9" t="n">
         <f aca="false">E19*F19</f>
-        <v>0</v>
+        <v>3.344</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>41</v>
@@ -1076,11 +1076,11 @@
       </c>
       <c r="F20" s="9" t="n">
         <f aca="false">$K$8</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G20" s="9" t="n">
         <f aca="false">E20*F20</f>
-        <v>0</v>
+        <v>0.0192</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>41</v>
@@ -1106,11 +1106,11 @@
       </c>
       <c r="F21" s="9" t="n">
         <f aca="false">$K$8</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G21" s="9" t="n">
         <f aca="false">E21*F21</f>
-        <v>0</v>
+        <v>0.0192</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>41</v>
@@ -1136,11 +1136,11 @@
       </c>
       <c r="F22" s="9" t="n">
         <f aca="false">$K$7*2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G22" s="9" t="n">
         <f aca="false">E22*F22</f>
-        <v>0</v>
+        <v>0.0216</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>22</v>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="G25" s="19" t="n">
         <f aca="false">SUM(G5:G24)</f>
-        <v>16.5349466666667</v>
+        <v>19.2740666666667</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>